<commit_message>
US 11 Notation Keys Functionality has been added.
</commit_message>
<xml_diff>
--- a/src/main/resources/ScenarioResults.xlsx
+++ b/src/main/resources/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="50">
   <si>
     <t>login-functionality;login-with-valid-username-and-password</t>
   </si>
@@ -108,6 +108,60 @@
   </si>
   <si>
     <t>2020-12-25 01_16_56</t>
+  </si>
+  <si>
+    <t>notation-functionalty;view-notation-keys-page</t>
+  </si>
+  <si>
+    <t>2021-01-01 15_39_05</t>
+  </si>
+  <si>
+    <t>notation-functionalty;create-a-new-notation-key</t>
+  </si>
+  <si>
+    <t>2021-01-01 15_39_33</t>
+  </si>
+  <si>
+    <t>notation-functionalty;edit-notation-key</t>
+  </si>
+  <si>
+    <t>2021-01-01 15_40_01</t>
+  </si>
+  <si>
+    <t>notation-functionalty;delete-the-notation-key</t>
+  </si>
+  <si>
+    <t>2021-01-01 15_40_26</t>
+  </si>
+  <si>
+    <t>2021-01-01 15_49_42</t>
+  </si>
+  <si>
+    <t>2021-01-01 15_50_11</t>
+  </si>
+  <si>
+    <t>2021-01-01 15_50_33</t>
+  </si>
+  <si>
+    <t>2021-01-01 15_51_03</t>
+  </si>
+  <si>
+    <t>2021-01-01 15_53_11</t>
+  </si>
+  <si>
+    <t>2021-01-01 15_54_37</t>
+  </si>
+  <si>
+    <t>2021-01-02 09_37_51</t>
+  </si>
+  <si>
+    <t>2021-01-02 09_38_22</t>
+  </si>
+  <si>
+    <t>2021-01-02 09_38_51</t>
+  </si>
+  <si>
+    <t>2021-01-02 09_39_16</t>
   </si>
 </sst>
 </file>
@@ -152,7 +206,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -494,6 +548,202 @@
         <v>3</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Dismissal Articles Test case ler tamamlandi.
</commit_message>
<xml_diff>
--- a/src/main/resources/ScenarioResults.xlsx
+++ b/src/main/resources/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="36">
   <si>
     <t>login-functionality;login-with-valid-username-and-password</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>2020-12-25 01_16_56</t>
+  </si>
+  <si>
+    <t>2021-01-01 17_23_50</t>
+  </si>
+  <si>
+    <t>2021-01-02 19_49_25</t>
+  </si>
+  <si>
+    <t>all-steps;step-by-step-from-dismissal-articles</t>
+  </si>
+  <si>
+    <t>2021-01-02 19_50_39</t>
   </si>
 </sst>
 </file>
@@ -152,7 +164,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -494,6 +506,48 @@
         <v>3</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>